<commit_message>
bindabasini mandir estimate given to shyam and kalimasta mandir estimate of temple shape to milan sir
</commit_message>
<xml_diff>
--- a/ofc/estimates/Finalized valuations/kalimasta mandir/milan sir.xlsx
+++ b/ofc/estimates/Finalized valuations/kalimasta mandir/milan sir.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\Finalized valuations\kalimasta mandir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\Finalized valuations\kalimasta mandir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'kalimasta mandir final (2)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -266,10 +266,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -435,7 +435,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -445,7 +445,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -465,14 +465,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -481,7 +481,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,7 +505,7 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -546,7 +546,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -561,7 +561,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -577,11 +577,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -597,30 +624,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -644,9 +647,6 @@
     </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1270,106 +1270,106 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="64" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="66" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="61" t="e">
+      <c r="C6" s="70" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1377,90 +1377,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="61" t="e">
+      <c r="J6" s="70" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="62"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="71"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="I7" s="71" t="s">
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="I7" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="69" t="e">
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="I8" s="72" t="s">
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="I8" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="73" t="e">
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="68" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="I9" s="72" t="s">
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="I9" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="67" t="s">
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74" t="s">
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="67" t="s">
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="68" t="s">
+      <c r="K11" s="63" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="62"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1479,10 +1479,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="67"/>
-      <c r="K12" s="68"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J12" s="62"/>
+      <c r="K12" s="63"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="32" t="e">
         <f>#REF!</f>
@@ -1547,7 +1547,7 @@
       <c r="J14" s="27"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="12"/>
@@ -1560,7 +1560,7 @@
       <c r="J15" s="27"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="12"/>
@@ -1616,7 +1616,7 @@
       <c r="J17" s="27"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -1642,6 +1642,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1655,13 +1662,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1679,135 +1679,135 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-    </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-    </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-    </row>
-    <row r="5" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-    </row>
-    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="69" t="s">
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="80" t="s">
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="81" t="s">
+      <c r="H7" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -1863,7 +1863,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="38" t="s">
         <v>47</v>
@@ -1895,7 +1895,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="38" t="s">
         <v>62</v>
@@ -1927,7 +1927,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="38" t="s">
         <v>48</v>
@@ -1959,7 +1959,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="38"/>
       <c r="C13" s="19">
@@ -1988,7 +1988,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="38" t="s">
         <v>59</v>
@@ -2019,7 +2019,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="38"/>
       <c r="C15" s="19">
@@ -2048,7 +2048,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="38" t="s">
         <v>60</v>
@@ -2080,7 +2080,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="38"/>
       <c r="C17" s="19">
@@ -2110,7 +2110,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="38" t="s">
         <v>61</v>
@@ -2142,7 +2142,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="38" t="s">
         <v>55</v>
@@ -2173,7 +2173,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="38" t="s">
         <v>58</v>
@@ -2204,7 +2204,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="38" t="s">
         <v>42</v>
@@ -2233,7 +2233,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="38" t="s">
         <v>40</v>
@@ -2255,7 +2255,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="38"/>
       <c r="C23" s="19"/>
@@ -2272,7 +2272,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>2</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="38" t="s">
         <v>47</v>
@@ -2323,7 +2323,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="38" t="s">
         <v>62</v>
@@ -2353,7 +2353,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="38" t="s">
         <v>48</v>
@@ -2383,7 +2383,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="38"/>
       <c r="C28" s="19">
@@ -2411,7 +2411,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="38" t="s">
         <v>59</v>
@@ -2441,7 +2441,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="38"/>
       <c r="C30" s="19">
@@ -2469,7 +2469,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="38" t="s">
         <v>60</v>
@@ -2500,7 +2500,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="38"/>
       <c r="C32" s="19">
@@ -2529,7 +2529,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="38" t="s">
         <v>61</v>
@@ -2558,7 +2558,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="38" t="s">
         <v>55</v>
@@ -2588,7 +2588,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="38" t="s">
         <v>58</v>
@@ -2618,7 +2618,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="38" t="s">
         <v>42</v>
@@ -2647,7 +2647,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="38" t="s">
         <v>40</v>
@@ -2669,7 +2669,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="38"/>
       <c r="C38" s="19"/>
@@ -2686,7 +2686,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="18">
         <v>3</v>
       </c>
@@ -2715,7 +2715,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="38" t="s">
         <v>53</v>
@@ -2749,7 +2749,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="38"/>
       <c r="C41" s="19">
@@ -2781,7 +2781,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="38"/>
       <c r="C42" s="19">
@@ -2813,7 +2813,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="38" t="s">
         <v>63</v>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="38"/>
       <c r="C44" s="19">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="38" t="s">
         <v>65</v>
@@ -2909,7 +2909,7 @@
         <v>0.39506172839506171</v>
       </c>
       <c r="F45" s="40">
-        <f>PRODUCT(C45:E45)</f>
+        <f t="shared" ref="F45:F59" si="11">PRODUCT(C45:E45)</f>
         <v>27.053827160493828</v>
       </c>
       <c r="G45" s="40">
@@ -2925,7 +2925,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="38" t="s">
         <v>64</v>
@@ -2943,11 +2943,11 @@
         <v>0.39506172839506171</v>
       </c>
       <c r="F46" s="40">
-        <f>PRODUCT(C46:E46)</f>
+        <f t="shared" si="11"/>
         <v>38.88987654320988</v>
       </c>
       <c r="G46" s="40">
-        <f t="shared" ref="G46:G48" si="11">F46/1000</f>
+        <f t="shared" ref="G46:G48" si="12">F46/1000</f>
         <v>3.8889876543209877E-2</v>
       </c>
       <c r="H46" s="22"/>
@@ -2959,7 +2959,7 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="38"/>
       <c r="C47" s="19">
@@ -2975,11 +2975,11 @@
         <v>0.39506172839506171</v>
       </c>
       <c r="F47" s="40">
-        <f>PRODUCT(C47:E47)</f>
+        <f t="shared" si="11"/>
         <v>27.25925925925926</v>
       </c>
       <c r="G47" s="40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7259259259259261E-2</v>
       </c>
       <c r="H47" s="22"/>
@@ -2991,7 +2991,7 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="38" t="s">
         <v>48</v>
@@ -3009,11 +3009,11 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="F48" s="40">
-        <f>PRODUCT(C48:E48)</f>
+        <f t="shared" si="11"/>
         <v>40.188289478140128</v>
       </c>
       <c r="G48" s="40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4.0188289478140127E-2</v>
       </c>
       <c r="H48" s="22"/>
@@ -3025,7 +3025,7 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="38"/>
       <c r="C49" s="19">
@@ -3041,11 +3041,11 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="F49" s="40">
-        <f>PRODUCT(C49:E49)</f>
+        <f t="shared" si="11"/>
         <v>39.51098919706051</v>
       </c>
       <c r="G49" s="40">
-        <f t="shared" ref="G49:G51" si="12">F49/1000</f>
+        <f t="shared" ref="G49:G51" si="13">F49/1000</f>
         <v>3.951098919706051E-2</v>
       </c>
       <c r="H49" s="22"/>
@@ -3057,7 +3057,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
       <c r="B50" s="38" t="s">
         <v>52</v>
@@ -3071,15 +3071,15 @@
         <v>0.81537945748247487</v>
       </c>
       <c r="E50" s="21">
-        <f t="shared" ref="E50:E51" si="13">8*8/162</f>
+        <f t="shared" ref="E50:E51" si="14">8*8/162</f>
         <v>0.39506172839506171</v>
       </c>
       <c r="F50" s="40">
-        <f>PRODUCT(C50:E50)</f>
+        <f t="shared" si="11"/>
         <v>9.341631315354773</v>
       </c>
       <c r="G50" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9.3416313153547731E-3</v>
       </c>
       <c r="H50" s="22"/>
@@ -3091,7 +3091,7 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
       <c r="B51" s="38"/>
       <c r="C51" s="19">
@@ -3103,15 +3103,15 @@
         <v>0.81537945748247487</v>
       </c>
       <c r="E51" s="21">
+        <f t="shared" si="14"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F51" s="40">
+        <f t="shared" si="11"/>
+        <v>9.0195060975839194</v>
+      </c>
+      <c r="G51" s="40">
         <f t="shared" si="13"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F51" s="40">
-        <f>PRODUCT(C51:E51)</f>
-        <v>9.0195060975839194</v>
-      </c>
-      <c r="G51" s="40">
-        <f t="shared" si="12"/>
         <v>9.0195060975839202E-3</v>
       </c>
       <c r="H51" s="22"/>
@@ -3123,7 +3123,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
       <c r="B52" s="38" t="s">
         <v>59</v>
@@ -3141,11 +3141,11 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="F52" s="40">
-        <f>PRODUCT(C52:E52)</f>
+        <f t="shared" si="11"/>
         <v>40.188289478140128</v>
       </c>
       <c r="G52" s="40">
-        <f t="shared" ref="G52" si="14">F52/1000</f>
+        <f t="shared" ref="G52" si="15">F52/1000</f>
         <v>4.0188289478140127E-2</v>
       </c>
       <c r="H52" s="22"/>
@@ -3157,7 +3157,7 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="18"/>
       <c r="B53" s="38"/>
       <c r="C53" s="19">
@@ -3173,11 +3173,11 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="F53" s="40">
-        <f>PRODUCT(C53:E53)</f>
+        <f t="shared" si="11"/>
         <v>39.51098919706051</v>
       </c>
       <c r="G53" s="40">
-        <f t="shared" ref="G53:G54" si="15">F53/1000</f>
+        <f t="shared" ref="G53:G54" si="16">F53/1000</f>
         <v>3.951098919706051E-2</v>
       </c>
       <c r="H53" s="22"/>
@@ -3189,7 +3189,7 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="18"/>
       <c r="B54" s="38" t="s">
         <v>52</v>
@@ -3203,15 +3203,15 @@
         <v>0.81537945748247487</v>
       </c>
       <c r="E54" s="21">
-        <f t="shared" ref="E54:E55" si="16">8*8/162</f>
+        <f t="shared" ref="E54:E55" si="17">8*8/162</f>
         <v>0.39506172839506171</v>
       </c>
       <c r="F54" s="40">
-        <f>PRODUCT(C54:E54)</f>
+        <f t="shared" si="11"/>
         <v>9.6637565331256265</v>
       </c>
       <c r="G54" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.663756533125626E-3</v>
       </c>
       <c r="H54" s="22"/>
@@ -3223,7 +3223,7 @@
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18"/>
       <c r="B55" s="38"/>
       <c r="C55" s="19">
@@ -3235,15 +3235,15 @@
         <v>0.81537945748247487</v>
       </c>
       <c r="E55" s="21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.39506172839506171</v>
       </c>
       <c r="F55" s="40">
-        <f>PRODUCT(C55:E55)</f>
+        <f t="shared" si="11"/>
         <v>9.6637565331256265</v>
       </c>
       <c r="G55" s="40">
-        <f t="shared" ref="G55" si="17">F55/1000</f>
+        <f t="shared" ref="G55" si="18">F55/1000</f>
         <v>9.663756533125626E-3</v>
       </c>
       <c r="H55" s="22"/>
@@ -3255,7 +3255,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18"/>
       <c r="B56" s="38" t="s">
         <v>60</v>
@@ -3273,11 +3273,11 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="F56" s="40">
-        <f>PRODUCT(C56:E56)</f>
+        <f t="shared" si="11"/>
         <v>28.901757594229394</v>
       </c>
       <c r="G56" s="40">
-        <f t="shared" ref="G56" si="18">F56/1000</f>
+        <f t="shared" ref="G56" si="19">F56/1000</f>
         <v>2.8901757594229395E-2</v>
       </c>
       <c r="H56" s="22"/>
@@ -3289,7 +3289,7 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
       <c r="B57" s="38"/>
       <c r="C57" s="19">
@@ -3305,11 +3305,11 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="F57" s="40">
-        <f>PRODUCT(C57:E57)</f>
+        <f t="shared" si="11"/>
         <v>28.901757594229394</v>
       </c>
       <c r="G57" s="40">
-        <f t="shared" ref="G57:G58" si="19">F57/1000</f>
+        <f t="shared" ref="G57:G58" si="20">F57/1000</f>
         <v>2.8901757594229395E-2</v>
       </c>
       <c r="H57" s="22"/>
@@ -3321,7 +3321,7 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18"/>
       <c r="B58" s="38" t="s">
         <v>52</v>
@@ -3335,15 +3335,15 @@
         <v>0.6</v>
       </c>
       <c r="E58" s="21">
-        <f t="shared" ref="E58" si="20">8*8/162</f>
+        <f t="shared" ref="E58" si="21">8*8/162</f>
         <v>0.39506172839506171</v>
       </c>
       <c r="F58" s="40">
-        <f>PRODUCT(C58:E58)</f>
+        <f t="shared" si="11"/>
         <v>15.170370370370369</v>
       </c>
       <c r="G58" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.5170370370370369E-2</v>
       </c>
       <c r="H58" s="22"/>
@@ -3355,7 +3355,7 @@
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18"/>
       <c r="B59" s="38" t="s">
         <v>61</v>
@@ -3373,11 +3373,11 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="F59" s="40">
-        <f>PRODUCT(C59:E59)</f>
+        <f t="shared" si="11"/>
         <v>34.677774391276365</v>
       </c>
       <c r="G59" s="40">
-        <f t="shared" ref="G59" si="21">F59/1000</f>
+        <f t="shared" ref="G59" si="22">F59/1000</f>
         <v>3.4677774391276367E-2</v>
       </c>
       <c r="H59" s="22"/>
@@ -3389,9 +3389,9 @@
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18"/>
-      <c r="B60" s="83" t="s">
+      <c r="B60" s="61" t="s">
         <v>66</v>
       </c>
       <c r="C60" s="19"/>
@@ -3411,7 +3411,7 @@
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18"/>
       <c r="B61" s="38" t="s">
         <v>42</v>
@@ -3440,7 +3440,7 @@
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="18"/>
       <c r="B62" s="38" t="s">
         <v>40</v>
@@ -3462,7 +3462,7 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18"/>
       <c r="B63" s="38"/>
       <c r="C63" s="19"/>
@@ -3479,7 +3479,7 @@
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18">
         <v>4</v>
       </c>
@@ -3493,7 +3493,7 @@
       <c r="E64" s="21"/>
       <c r="F64" s="21"/>
       <c r="G64" s="33">
-        <f t="shared" ref="G64" si="22">PRODUCT(C64:F64)</f>
+        <f t="shared" ref="G64" si="23">PRODUCT(C64:F64)</f>
         <v>1</v>
       </c>
       <c r="H64" s="22" t="s">
@@ -3512,7 +3512,7 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18"/>
       <c r="B65" s="24"/>
       <c r="C65" s="19"/>
@@ -3529,7 +3529,7 @@
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="41"/>
       <c r="B66" s="43" t="s">
         <v>17</v>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="K66" s="37"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="55"/>
       <c r="B67" s="58"/>
       <c r="C67" s="59"/>
@@ -3560,16 +3560,16 @@
       <c r="J67" s="57"/>
       <c r="K67" s="54"/>
     </row>
-    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="47"/>
       <c r="B68" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C68" s="79">
+      <c r="C68" s="80">
         <f>J66</f>
         <v>483837.72404040786</v>
       </c>
-      <c r="D68" s="79"/>
+      <c r="D68" s="80"/>
       <c r="E68" s="40">
         <v>100</v>
       </c>
@@ -3580,15 +3580,15 @@
       <c r="J68" s="51"/>
       <c r="K68" s="52"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="53"/>
       <c r="B69" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C69" s="82">
+      <c r="C69" s="83">
         <v>430000</v>
       </c>
-      <c r="D69" s="82"/>
+      <c r="D69" s="83"/>
       <c r="E69" s="40"/>
       <c r="F69" s="46"/>
       <c r="G69" s="45"/>
@@ -3597,16 +3597,16 @@
       <c r="J69" s="45"/>
       <c r="K69" s="46"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="53"/>
       <c r="B70" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="82">
+      <c r="C70" s="83">
         <f>C69-C72-C73</f>
         <v>408500</v>
       </c>
-      <c r="D70" s="82"/>
+      <c r="D70" s="83"/>
       <c r="E70" s="40">
         <f>C70/C68*100</f>
         <v>84.429133922985301</v>
@@ -3618,16 +3618,16 @@
       <c r="J70" s="45"/>
       <c r="K70" s="46"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="53"/>
       <c r="B71" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C71" s="79">
+      <c r="C71" s="80">
         <f>C68-C70</f>
         <v>75337.724040407862</v>
       </c>
-      <c r="D71" s="79"/>
+      <c r="D71" s="80"/>
       <c r="E71" s="40">
         <f>100-E70</f>
         <v>15.570866077014699</v>
@@ -3639,16 +3639,16 @@
       <c r="J71" s="45"/>
       <c r="K71" s="46"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="53"/>
       <c r="B72" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C72" s="79">
+      <c r="C72" s="80">
         <f>C69*0.03</f>
         <v>12900</v>
       </c>
-      <c r="D72" s="79"/>
+      <c r="D72" s="80"/>
       <c r="E72" s="40">
         <v>3</v>
       </c>
@@ -3659,16 +3659,16 @@
       <c r="J72" s="45"/>
       <c r="K72" s="46"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="53"/>
       <c r="B73" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C73" s="79">
+      <c r="C73" s="80">
         <f>C69*0.02</f>
         <v>8600</v>
       </c>
-      <c r="D73" s="79"/>
+      <c r="D73" s="80"/>
       <c r="E73" s="40">
         <v>2</v>
       </c>
@@ -3679,7 +3679,7 @@
       <c r="J73" s="45"/>
       <c r="K73" s="46"/>
     </row>
-    <row r="74" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="54"/>
       <c r="B74" s="54"/>
       <c r="C74" s="54"/>
@@ -3692,71 +3692,64 @@
       <c r="J74" s="54"/>
       <c r="K74" s="54"/>
     </row>
-    <row r="75" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="C73:D73"/>
     <mergeCell ref="A7:F7"/>
@@ -3765,6 +3758,13 @@
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="C71:D71"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>